<commit_message>
Use MEURyyyy instead of EURyy
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\times-ireland-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF76D145-6C77-451A-8F59-9CDFA2CB17DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F4301C-F6E1-47DB-AF32-B6B8F053848E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32160" yWindow="2475" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="28" r:id="rId1"/>
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="173">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -306,12 +306,6 @@
   </si>
   <si>
     <t>P12</t>
-  </si>
-  <si>
-    <t>EUR18</t>
-  </si>
-  <si>
-    <t>EUR19</t>
   </si>
   <si>
     <t>Development</t>
@@ -593,9 +587,6 @@
     <t>P23</t>
   </si>
   <si>
-    <t>EUR20</t>
-  </si>
-  <si>
     <t>SRV</t>
   </si>
   <si>
@@ -657,6 +648,9 @@
   </si>
   <si>
     <t>James Glynn (UCC, james.glynn@ucc.ie)</t>
+  </si>
+  <si>
+    <t>MEUR2018</t>
   </si>
 </sst>
 </file>
@@ -4260,23 +4254,25 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:Z99"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="4" width="21.7109375" style="44" customWidth="1"/>
-    <col min="5" max="6" width="14.140625" style="44" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="44" customWidth="1"/>
-    <col min="8" max="10" width="8.140625" style="44" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" style="44" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" style="44" customWidth="1"/>
+    <col min="1" max="4" width="21.73046875" style="44" customWidth="1"/>
+    <col min="5" max="6" width="14.1328125" style="44" customWidth="1"/>
+    <col min="7" max="7" width="12.1328125" style="44" customWidth="1"/>
+    <col min="8" max="10" width="8.1328125" style="44" customWidth="1"/>
+    <col min="11" max="11" width="9.73046875" style="44" customWidth="1"/>
+    <col min="12" max="12" width="8.1328125" style="44" customWidth="1"/>
     <col min="13" max="13" width="10" style="44" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" style="44" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" style="44" customWidth="1"/>
-    <col min="16" max="16384" width="8.85546875" style="44"/>
+    <col min="14" max="14" width="11.3984375" style="44" customWidth="1"/>
+    <col min="15" max="15" width="13.3984375" style="44" customWidth="1"/>
+    <col min="16" max="16384" width="8.86328125" style="44"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A1" s="42"/>
       <c r="B1" s="42"/>
       <c r="C1" s="42"/>
@@ -4304,7 +4300,7 @@
       <c r="Y1" s="43"/>
       <c r="Z1" s="43"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A2" s="42"/>
       <c r="B2" s="42"/>
       <c r="C2" s="42"/>
@@ -4332,7 +4328,7 @@
       <c r="Y2" s="43"/>
       <c r="Z2" s="43"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A3" s="42"/>
       <c r="B3" s="42"/>
       <c r="C3" s="42"/>
@@ -4360,7 +4356,7 @@
       <c r="Y3" s="43"/>
       <c r="Z3" s="43"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A4" s="42"/>
       <c r="B4" s="42"/>
       <c r="C4" s="42"/>
@@ -4388,7 +4384,7 @@
       <c r="Y4" s="43"/>
       <c r="Z4" s="43"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A5" s="42"/>
       <c r="B5" s="42"/>
       <c r="C5" s="42"/>
@@ -4416,7 +4412,7 @@
       <c r="Y5" s="43"/>
       <c r="Z5" s="43"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A6" s="42"/>
       <c r="B6" s="42"/>
       <c r="C6" s="42"/>
@@ -4444,7 +4440,7 @@
       <c r="Y6" s="43"/>
       <c r="Z6" s="43"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A7" s="42"/>
       <c r="B7" s="42"/>
       <c r="C7" s="42"/>
@@ -4472,7 +4468,7 @@
       <c r="Y7" s="43"/>
       <c r="Z7" s="43"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A8" s="42"/>
       <c r="B8" s="42"/>
       <c r="C8" s="42"/>
@@ -4500,7 +4496,7 @@
       <c r="Y8" s="43"/>
       <c r="Z8" s="43"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A9" s="42"/>
       <c r="B9" s="42"/>
       <c r="C9" s="42"/>
@@ -4528,7 +4524,7 @@
       <c r="Y9" s="43"/>
       <c r="Z9" s="43"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A10" s="42"/>
       <c r="B10" s="42"/>
       <c r="C10" s="42"/>
@@ -4556,7 +4552,7 @@
       <c r="Y10" s="43"/>
       <c r="Z10" s="43"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A11" s="42"/>
       <c r="B11" s="42"/>
       <c r="C11" s="42"/>
@@ -4584,7 +4580,7 @@
       <c r="Y11" s="43"/>
       <c r="Z11" s="43"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A12" s="42"/>
       <c r="B12" s="42"/>
       <c r="C12" s="42"/>
@@ -4612,7 +4608,7 @@
       <c r="Y12" s="43"/>
       <c r="Z12" s="43"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A13" s="42"/>
       <c r="B13" s="42"/>
       <c r="C13" s="42"/>
@@ -4640,7 +4636,7 @@
       <c r="Y13" s="43"/>
       <c r="Z13" s="43"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A14" s="42"/>
       <c r="B14" s="42"/>
       <c r="C14" s="42"/>
@@ -4668,7 +4664,7 @@
       <c r="Y14" s="43"/>
       <c r="Z14" s="43"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A15" s="42"/>
       <c r="B15" s="42"/>
       <c r="C15" s="42"/>
@@ -4696,9 +4692,9 @@
       <c r="Y15" s="43"/>
       <c r="Z15" s="43"/>
     </row>
-    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="59" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B16" s="59"/>
       <c r="C16" s="59"/>
@@ -4726,7 +4722,7 @@
       <c r="Y16" s="43"/>
       <c r="Z16" s="43"/>
     </row>
-    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="47"/>
       <c r="B17" s="47"/>
       <c r="C17" s="47"/>
@@ -4754,7 +4750,7 @@
       <c r="Y17" s="43"/>
       <c r="Z17" s="43"/>
     </row>
-    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="47"/>
       <c r="B18" s="47"/>
       <c r="C18" s="47"/>
@@ -4782,12 +4778,12 @@
       <c r="Y18" s="43"/>
       <c r="Z18" s="43"/>
     </row>
-    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="50" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B19" s="58" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C19" s="58"/>
       <c r="D19" s="58"/>
@@ -4814,12 +4810,12 @@
       <c r="Y19" s="43"/>
       <c r="Z19" s="43"/>
     </row>
-    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="50" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B20" s="58" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C20" s="58"/>
       <c r="D20" s="58"/>
@@ -4846,12 +4842,12 @@
       <c r="Y20" s="43"/>
       <c r="Z20" s="43"/>
     </row>
-    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="50" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B21" s="53" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C21" s="53"/>
       <c r="D21" s="53"/>
@@ -4878,7 +4874,7 @@
       <c r="Y21" s="43"/>
       <c r="Z21" s="43"/>
     </row>
-    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="50"/>
       <c r="B22" s="53"/>
       <c r="C22" s="53"/>
@@ -4906,12 +4902,12 @@
       <c r="Y22" s="43"/>
       <c r="Z22" s="43"/>
     </row>
-    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="50" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B23" s="58" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C23" s="58"/>
       <c r="D23" s="58"/>
@@ -4938,7 +4934,7 @@
       <c r="Y23" s="43"/>
       <c r="Z23" s="43"/>
     </row>
-    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="50"/>
       <c r="B24" s="53"/>
       <c r="C24" s="53"/>
@@ -4966,7 +4962,7 @@
       <c r="Y24" s="43"/>
       <c r="Z24" s="43"/>
     </row>
-    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="50"/>
       <c r="B25" s="53"/>
       <c r="C25" s="53"/>
@@ -4994,12 +4990,12 @@
       <c r="Y25" s="43"/>
       <c r="Z25" s="43"/>
     </row>
-    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="50" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B26" s="58" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C26" s="58"/>
       <c r="D26" s="58"/>
@@ -5026,7 +5022,7 @@
       <c r="Y26" s="43"/>
       <c r="Z26" s="43"/>
     </row>
-    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="50"/>
       <c r="B27" s="53"/>
       <c r="C27" s="53"/>
@@ -5054,7 +5050,7 @@
       <c r="Y27" s="43"/>
       <c r="Z27" s="43"/>
     </row>
-    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="50"/>
       <c r="B28" s="53"/>
       <c r="C28" s="53"/>
@@ -5082,9 +5078,9 @@
       <c r="Y28" s="43"/>
       <c r="Z28" s="43"/>
     </row>
-    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="50" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B29" s="54">
         <v>1</v>
@@ -5114,12 +5110,12 @@
       <c r="Y29" s="43"/>
       <c r="Z29" s="43"/>
     </row>
-    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="50" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B30" s="60" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C30" s="58"/>
       <c r="D30" s="58"/>
@@ -5146,12 +5142,12 @@
       <c r="Y30" s="43"/>
       <c r="Z30" s="43"/>
     </row>
-    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="50" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B31" s="58" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C31" s="58"/>
       <c r="D31" s="58"/>
@@ -5178,10 +5174,10 @@
       <c r="Y31" s="43"/>
       <c r="Z31" s="43"/>
     </row>
-    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="56"/>
       <c r="B32" s="57" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C32" s="56"/>
       <c r="D32" s="56"/>
@@ -5208,7 +5204,7 @@
       <c r="Y32" s="43"/>
       <c r="Z32" s="43"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A33" s="42"/>
       <c r="B33" s="42"/>
       <c r="C33" s="42"/>
@@ -5236,7 +5232,7 @@
       <c r="Y33" s="43"/>
       <c r="Z33" s="43"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A34" s="42"/>
       <c r="B34" s="42"/>
       <c r="C34" s="42"/>
@@ -5264,7 +5260,7 @@
       <c r="Y34" s="43"/>
       <c r="Z34" s="43"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A35" s="42"/>
       <c r="B35" s="42"/>
       <c r="C35" s="42"/>
@@ -5292,7 +5288,7 @@
       <c r="Y35" s="43"/>
       <c r="Z35" s="43"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A36" s="42"/>
       <c r="B36" s="42"/>
       <c r="C36" s="42"/>
@@ -5320,7 +5316,7 @@
       <c r="Y36" s="43"/>
       <c r="Z36" s="43"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A37" s="42"/>
       <c r="B37" s="42"/>
       <c r="C37" s="42"/>
@@ -5348,7 +5344,7 @@
       <c r="Y37" s="43"/>
       <c r="Z37" s="43"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A38" s="42"/>
       <c r="B38" s="42"/>
       <c r="C38" s="42"/>
@@ -5376,7 +5372,7 @@
       <c r="Y38" s="43"/>
       <c r="Z38" s="43"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A39" s="42"/>
       <c r="B39" s="42"/>
       <c r="C39" s="42"/>
@@ -5404,7 +5400,7 @@
       <c r="Y39" s="43"/>
       <c r="Z39" s="43"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A40" s="42"/>
       <c r="B40" s="42"/>
       <c r="C40" s="42"/>
@@ -5432,7 +5428,7 @@
       <c r="Y40" s="43"/>
       <c r="Z40" s="43"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A41" s="42"/>
       <c r="B41" s="42"/>
       <c r="C41" s="42"/>
@@ -5460,7 +5456,7 @@
       <c r="Y41" s="43"/>
       <c r="Z41" s="43"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A42" s="42"/>
       <c r="B42" s="42"/>
       <c r="C42" s="42"/>
@@ -5488,7 +5484,7 @@
       <c r="Y42" s="43"/>
       <c r="Z42" s="43"/>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A43" s="43"/>
       <c r="B43" s="43"/>
       <c r="C43" s="43"/>
@@ -5516,7 +5512,7 @@
       <c r="Y43" s="43"/>
       <c r="Z43" s="43"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A44" s="43"/>
       <c r="B44" s="43"/>
       <c r="C44" s="43"/>
@@ -5544,7 +5540,7 @@
       <c r="Y44" s="43"/>
       <c r="Z44" s="43"/>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A45" s="43"/>
       <c r="B45" s="43"/>
       <c r="C45" s="43"/>
@@ -5572,7 +5568,7 @@
       <c r="Y45" s="43"/>
       <c r="Z45" s="43"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A46" s="43"/>
       <c r="B46" s="43"/>
       <c r="C46" s="43"/>
@@ -5600,7 +5596,7 @@
       <c r="Y46" s="43"/>
       <c r="Z46" s="43"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A47" s="43"/>
       <c r="B47" s="43"/>
       <c r="C47" s="43"/>
@@ -5628,7 +5624,7 @@
       <c r="Y47" s="43"/>
       <c r="Z47" s="43"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A48" s="43"/>
       <c r="B48" s="43"/>
       <c r="C48" s="43"/>
@@ -5656,7 +5652,7 @@
       <c r="Y48" s="43"/>
       <c r="Z48" s="43"/>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A49" s="43"/>
       <c r="B49" s="43"/>
       <c r="C49" s="43"/>
@@ -5684,7 +5680,7 @@
       <c r="Y49" s="43"/>
       <c r="Z49" s="43"/>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A50" s="43"/>
       <c r="B50" s="43"/>
       <c r="C50" s="43"/>
@@ -5712,7 +5708,7 @@
       <c r="Y50" s="43"/>
       <c r="Z50" s="43"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A51" s="43"/>
       <c r="B51" s="43"/>
       <c r="C51" s="43"/>
@@ -5740,7 +5736,7 @@
       <c r="Y51" s="43"/>
       <c r="Z51" s="43"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A52" s="43"/>
       <c r="B52" s="43"/>
       <c r="C52" s="43"/>
@@ -5768,7 +5764,7 @@
       <c r="Y52" s="43"/>
       <c r="Z52" s="43"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A53" s="43"/>
       <c r="B53" s="43"/>
       <c r="C53" s="43"/>
@@ -5796,7 +5792,7 @@
       <c r="Y53" s="43"/>
       <c r="Z53" s="43"/>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A54" s="43"/>
       <c r="B54" s="43"/>
       <c r="C54" s="43"/>
@@ -5824,7 +5820,7 @@
       <c r="Y54" s="43"/>
       <c r="Z54" s="43"/>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A55" s="43"/>
       <c r="B55" s="43"/>
       <c r="C55" s="43"/>
@@ -5852,7 +5848,7 @@
       <c r="Y55" s="43"/>
       <c r="Z55" s="43"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A56" s="43"/>
       <c r="B56" s="43"/>
       <c r="C56" s="43"/>
@@ -5880,7 +5876,7 @@
       <c r="Y56" s="43"/>
       <c r="Z56" s="43"/>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A57" s="43"/>
       <c r="B57" s="43"/>
       <c r="C57" s="43"/>
@@ -5908,7 +5904,7 @@
       <c r="Y57" s="43"/>
       <c r="Z57" s="43"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A58" s="43"/>
       <c r="B58" s="43"/>
       <c r="C58" s="43"/>
@@ -5936,7 +5932,7 @@
       <c r="Y58" s="43"/>
       <c r="Z58" s="43"/>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A59" s="43"/>
       <c r="B59" s="43"/>
       <c r="C59" s="43"/>
@@ -5964,7 +5960,7 @@
       <c r="Y59" s="43"/>
       <c r="Z59" s="43"/>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A60" s="43"/>
       <c r="B60" s="43"/>
       <c r="C60" s="43"/>
@@ -5992,7 +5988,7 @@
       <c r="Y60" s="43"/>
       <c r="Z60" s="43"/>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A61" s="43"/>
       <c r="B61" s="43"/>
       <c r="C61" s="43"/>
@@ -6020,7 +6016,7 @@
       <c r="Y61" s="43"/>
       <c r="Z61" s="43"/>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A62" s="43"/>
       <c r="B62" s="43"/>
       <c r="C62" s="43"/>
@@ -6048,7 +6044,7 @@
       <c r="Y62" s="43"/>
       <c r="Z62" s="43"/>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A63" s="43"/>
       <c r="B63" s="43"/>
       <c r="C63" s="43"/>
@@ -6076,7 +6072,7 @@
       <c r="Y63" s="43"/>
       <c r="Z63" s="43"/>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A64" s="43"/>
       <c r="B64" s="43"/>
       <c r="C64" s="43"/>
@@ -6104,7 +6100,7 @@
       <c r="Y64" s="43"/>
       <c r="Z64" s="43"/>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A65" s="43"/>
       <c r="B65" s="43"/>
       <c r="C65" s="43"/>
@@ -6132,7 +6128,7 @@
       <c r="Y65" s="43"/>
       <c r="Z65" s="43"/>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A66" s="43"/>
       <c r="B66" s="43"/>
       <c r="C66" s="43"/>
@@ -6160,7 +6156,7 @@
       <c r="Y66" s="43"/>
       <c r="Z66" s="43"/>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A67" s="43"/>
       <c r="B67" s="43"/>
       <c r="C67" s="43"/>
@@ -6188,7 +6184,7 @@
       <c r="Y67" s="43"/>
       <c r="Z67" s="43"/>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A68" s="43"/>
       <c r="B68" s="43"/>
       <c r="C68" s="43"/>
@@ -6216,7 +6212,7 @@
       <c r="Y68" s="43"/>
       <c r="Z68" s="43"/>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A69" s="43"/>
       <c r="B69" s="43"/>
       <c r="C69" s="43"/>
@@ -6244,7 +6240,7 @@
       <c r="Y69" s="43"/>
       <c r="Z69" s="43"/>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A70" s="43"/>
       <c r="B70" s="43"/>
       <c r="C70" s="43"/>
@@ -6272,7 +6268,7 @@
       <c r="Y70" s="43"/>
       <c r="Z70" s="43"/>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A71" s="43"/>
       <c r="B71" s="43"/>
       <c r="C71" s="43"/>
@@ -6300,7 +6296,7 @@
       <c r="Y71" s="43"/>
       <c r="Z71" s="43"/>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A72" s="43"/>
       <c r="B72" s="43"/>
       <c r="C72" s="43"/>
@@ -6328,7 +6324,7 @@
       <c r="Y72" s="43"/>
       <c r="Z72" s="43"/>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A73" s="43"/>
       <c r="B73" s="43"/>
       <c r="C73" s="43"/>
@@ -6356,7 +6352,7 @@
       <c r="Y73" s="43"/>
       <c r="Z73" s="43"/>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A74" s="43"/>
       <c r="B74" s="43"/>
       <c r="C74" s="43"/>
@@ -6384,7 +6380,7 @@
       <c r="Y74" s="43"/>
       <c r="Z74" s="43"/>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A75" s="43"/>
       <c r="B75" s="43"/>
       <c r="C75" s="43"/>
@@ -6412,7 +6408,7 @@
       <c r="Y75" s="43"/>
       <c r="Z75" s="43"/>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A76" s="43"/>
       <c r="B76" s="43"/>
       <c r="C76" s="43"/>
@@ -6440,7 +6436,7 @@
       <c r="Y76" s="43"/>
       <c r="Z76" s="43"/>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A77" s="43"/>
       <c r="B77" s="43"/>
       <c r="C77" s="43"/>
@@ -6468,7 +6464,7 @@
       <c r="Y77" s="43"/>
       <c r="Z77" s="43"/>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A78" s="43"/>
       <c r="B78" s="43"/>
       <c r="C78" s="43"/>
@@ -6496,7 +6492,7 @@
       <c r="Y78" s="43"/>
       <c r="Z78" s="43"/>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A79" s="43"/>
       <c r="B79" s="43"/>
       <c r="C79" s="43"/>
@@ -6524,7 +6520,7 @@
       <c r="Y79" s="43"/>
       <c r="Z79" s="43"/>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A80" s="43"/>
       <c r="B80" s="43"/>
       <c r="C80" s="43"/>
@@ -6552,7 +6548,7 @@
       <c r="Y80" s="43"/>
       <c r="Z80" s="43"/>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A81" s="43"/>
       <c r="B81" s="43"/>
       <c r="C81" s="43"/>
@@ -6580,7 +6576,7 @@
       <c r="Y81" s="43"/>
       <c r="Z81" s="43"/>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A82" s="43"/>
       <c r="B82" s="43"/>
       <c r="C82" s="43"/>
@@ -6608,7 +6604,7 @@
       <c r="Y82" s="43"/>
       <c r="Z82" s="43"/>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A83" s="43"/>
       <c r="B83" s="43"/>
       <c r="C83" s="43"/>
@@ -6636,7 +6632,7 @@
       <c r="Y83" s="43"/>
       <c r="Z83" s="43"/>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A84" s="43"/>
       <c r="B84" s="43"/>
       <c r="C84" s="43"/>
@@ -6664,7 +6660,7 @@
       <c r="Y84" s="43"/>
       <c r="Z84" s="43"/>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A85" s="43"/>
       <c r="B85" s="43"/>
       <c r="C85" s="43"/>
@@ -6692,7 +6688,7 @@
       <c r="Y85" s="43"/>
       <c r="Z85" s="43"/>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A86" s="43"/>
       <c r="B86" s="43"/>
       <c r="C86" s="43"/>
@@ -6720,7 +6716,7 @@
       <c r="Y86" s="43"/>
       <c r="Z86" s="43"/>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A87" s="43"/>
       <c r="B87" s="43"/>
       <c r="C87" s="43"/>
@@ -6748,7 +6744,7 @@
       <c r="Y87" s="43"/>
       <c r="Z87" s="43"/>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A88" s="43"/>
       <c r="B88" s="43"/>
       <c r="C88" s="43"/>
@@ -6776,7 +6772,7 @@
       <c r="Y88" s="43"/>
       <c r="Z88" s="43"/>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A89" s="43"/>
       <c r="B89" s="43"/>
       <c r="C89" s="43"/>
@@ -6804,7 +6800,7 @@
       <c r="Y89" s="43"/>
       <c r="Z89" s="43"/>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A90" s="43"/>
       <c r="B90" s="43"/>
       <c r="C90" s="43"/>
@@ -6832,7 +6828,7 @@
       <c r="Y90" s="43"/>
       <c r="Z90" s="43"/>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A91" s="43"/>
       <c r="B91" s="43"/>
       <c r="C91" s="43"/>
@@ -6860,7 +6856,7 @@
       <c r="Y91" s="43"/>
       <c r="Z91" s="43"/>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A92" s="43"/>
       <c r="B92" s="43"/>
       <c r="C92" s="43"/>
@@ -6888,7 +6884,7 @@
       <c r="Y92" s="43"/>
       <c r="Z92" s="43"/>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A93" s="43"/>
       <c r="B93" s="43"/>
       <c r="C93" s="43"/>
@@ -6916,7 +6912,7 @@
       <c r="Y93" s="43"/>
       <c r="Z93" s="43"/>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A94" s="43"/>
       <c r="B94" s="43"/>
       <c r="C94" s="43"/>
@@ -6944,7 +6940,7 @@
       <c r="Y94" s="43"/>
       <c r="Z94" s="43"/>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A95" s="43"/>
       <c r="B95" s="43"/>
       <c r="C95" s="43"/>
@@ -6972,7 +6968,7 @@
       <c r="Y95" s="43"/>
       <c r="Z95" s="43"/>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A96" s="43"/>
       <c r="B96" s="43"/>
       <c r="C96" s="43"/>
@@ -7000,7 +6996,7 @@
       <c r="Y96" s="43"/>
       <c r="Z96" s="43"/>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A97" s="43"/>
       <c r="B97" s="43"/>
       <c r="C97" s="43"/>
@@ -7028,7 +7024,7 @@
       <c r="Y97" s="43"/>
       <c r="Z97" s="43"/>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A98" s="43"/>
       <c r="B98" s="43"/>
       <c r="C98" s="43"/>
@@ -7056,7 +7052,7 @@
       <c r="Y98" s="43"/>
       <c r="Z98" s="43"/>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A99" s="43"/>
       <c r="B99" s="43"/>
       <c r="C99" s="43"/>
@@ -7113,38 +7109,38 @@
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="3.140625" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" customWidth="1"/>
+    <col min="1" max="1" width="12.1328125" customWidth="1"/>
+    <col min="2" max="2" width="11.73046875" customWidth="1"/>
+    <col min="3" max="3" width="3.1328125" customWidth="1"/>
+    <col min="4" max="4" width="8.59765625" customWidth="1"/>
+    <col min="5" max="5" width="6.3984375" customWidth="1"/>
     <col min="6" max="6" width="5" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" customWidth="1"/>
-    <col min="8" max="8" width="5.85546875" customWidth="1"/>
-    <col min="9" max="9" width="5.42578125" customWidth="1"/>
-    <col min="10" max="11" width="5.7109375" customWidth="1"/>
-    <col min="12" max="12" width="6.5703125" customWidth="1"/>
+    <col min="7" max="7" width="5.73046875" customWidth="1"/>
+    <col min="8" max="8" width="5.86328125" customWidth="1"/>
+    <col min="9" max="9" width="5.3984375" customWidth="1"/>
+    <col min="10" max="11" width="5.73046875" customWidth="1"/>
+    <col min="12" max="12" width="6.59765625" customWidth="1"/>
     <col min="13" max="13" width="6" customWidth="1"/>
-    <col min="14" max="14" width="6.7109375" customWidth="1"/>
-    <col min="15" max="15" width="6.5703125" customWidth="1"/>
-    <col min="16" max="16" width="7.140625" customWidth="1"/>
-    <col min="17" max="17" width="5.7109375" customWidth="1"/>
+    <col min="14" max="14" width="6.73046875" customWidth="1"/>
+    <col min="15" max="15" width="6.59765625" customWidth="1"/>
+    <col min="16" max="16" width="7.1328125" customWidth="1"/>
+    <col min="17" max="17" width="5.73046875" customWidth="1"/>
     <col min="18" max="18" width="6" customWidth="1"/>
-    <col min="19" max="19" width="5.85546875" customWidth="1"/>
-    <col min="20" max="20" width="5.5703125" customWidth="1"/>
-    <col min="21" max="21" width="5.85546875" customWidth="1"/>
-    <col min="22" max="22" width="6.7109375" customWidth="1"/>
+    <col min="19" max="19" width="5.86328125" customWidth="1"/>
+    <col min="20" max="20" width="5.59765625" customWidth="1"/>
+    <col min="21" max="21" width="5.86328125" customWidth="1"/>
+    <col min="22" max="22" width="6.73046875" customWidth="1"/>
     <col min="23" max="23" width="5" customWidth="1"/>
-    <col min="24" max="24" width="7.5703125" customWidth="1"/>
-    <col min="25" max="25" width="6.7109375" customWidth="1"/>
+    <col min="24" max="24" width="7.59765625" customWidth="1"/>
+    <col min="25" max="25" width="6.73046875" customWidth="1"/>
     <col min="26" max="28" width="6" customWidth="1"/>
-    <col min="29" max="29" width="5.7109375" customWidth="1"/>
-    <col min="30" max="30" width="6.7109375" customWidth="1"/>
+    <col min="29" max="29" width="5.73046875" customWidth="1"/>
+    <col min="30" max="30" width="6.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C3" s="2" t="str">
         <f t="array" ref="C3">IF(INDEX(C5:C7,$A$4)&lt;&gt;0,INDEX(C5:C7,$A$4),"")</f>
         <v>IE</v>
@@ -7258,21 +7254,21 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>1</v>
       </c>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E5" s="2" t="str">
         <f>A11</f>
@@ -7379,9 +7375,9 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C6" s="2" t="str">
         <f>C5</f>
@@ -7415,9 +7411,9 @@
       <c r="AC6" s="2"/>
       <c r="AD6" s="2"/>
     </row>
-    <row r="7" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C7" s="2" t="str">
         <f t="shared" ref="C7:AC7" si="0">D5</f>
@@ -7529,225 +7525,225 @@
       </c>
       <c r="AD7" s="2"/>
     </row>
-    <row r="10" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B12" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B13" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B14" s="5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B15" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B16" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B17" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B18" s="5" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B19" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B20" s="5" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B21" s="5" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B22" s="5" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B23" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B24" s="5" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B25" s="5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B26" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B27" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B28" s="5" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B29" s="5" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B30" s="5" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="5" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B31" s="5" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="5" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B32" s="5" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="5" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B33" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="5" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B34" s="5" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="5" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B35" s="5" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="5" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B36" s="5" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="5" t="s">
+    <row r="37" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A37" s="6" t="s">
         <v>122</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
-        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -7791,20 +7787,20 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A3:AB39"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T25" sqref="T25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.140625" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="2.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="2.1328125" customWidth="1"/>
+    <col min="2" max="2" width="19.1328125" customWidth="1"/>
+    <col min="4" max="4" width="2.1328125" customWidth="1"/>
+    <col min="5" max="5" width="12.1328125" customWidth="1"/>
+    <col min="6" max="6" width="13.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A3" s="7"/>
       <c r="B3" s="11" t="s">
         <v>6</v>
@@ -7815,7 +7811,7 @@
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="7"/>
       <c r="B4" s="9" t="s">
         <v>12</v>
@@ -7833,25 +7829,25 @@
         <v>11</v>
       </c>
       <c r="K4" t="s">
+        <v>124</v>
+      </c>
+      <c r="L4" t="s">
+        <v>125</v>
+      </c>
+      <c r="N4" t="s">
         <v>126</v>
       </c>
-      <c r="L4" t="s">
+      <c r="O4" t="s">
         <v>127</v>
       </c>
-      <c r="N4" t="s">
+      <c r="Q4" t="s">
         <v>128</v>
       </c>
-      <c r="O4" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>130</v>
-      </c>
       <c r="R4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A5" s="7"/>
       <c r="B5" s="8" t="s">
         <v>37</v>
@@ -7861,34 +7857,34 @@
         <v>IE</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
       <c r="L5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N5">
         <v>0</v>
       </c>
       <c r="O5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="Q5">
         <v>0</v>
       </c>
       <c r="R5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8" t="str">
@@ -7902,22 +7898,22 @@
         <v>1</v>
       </c>
       <c r="L6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N6">
         <v>1</v>
       </c>
       <c r="O6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="Q6">
         <v>1</v>
       </c>
       <c r="R6" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="8" t="str">
@@ -7931,22 +7927,22 @@
         <v>2</v>
       </c>
       <c r="L7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N7">
         <v>2</v>
       </c>
       <c r="O7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="Q7">
         <v>2</v>
       </c>
       <c r="R7" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="8" t="str">
@@ -7960,22 +7956,22 @@
         <v>3</v>
       </c>
       <c r="L8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N8">
         <v>3</v>
       </c>
       <c r="O8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="Q8">
         <v>3</v>
       </c>
       <c r="R8" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="8" t="str">
@@ -7986,22 +7982,22 @@
         <v>4</v>
       </c>
       <c r="L9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N9">
         <v>4</v>
       </c>
       <c r="O9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="Q9">
         <v>4</v>
       </c>
       <c r="R9" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="8" t="str">
@@ -8012,22 +8008,22 @@
         <v>5</v>
       </c>
       <c r="L10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N10">
         <v>5</v>
       </c>
       <c r="O10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="Q10">
         <v>5</v>
       </c>
       <c r="R10" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="8" t="str">
@@ -8039,22 +8035,22 @@
         <v>6</v>
       </c>
       <c r="L11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N11">
         <v>6</v>
       </c>
       <c r="O11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="Q11">
         <v>6</v>
       </c>
       <c r="R11" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="8" t="str">
@@ -8066,16 +8062,16 @@
         <v>7</v>
       </c>
       <c r="L12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="Q12">
         <v>7</v>
       </c>
       <c r="R12" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="8" t="str">
@@ -8087,16 +8083,16 @@
         <v>8</v>
       </c>
       <c r="L13" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="Q13">
         <v>8</v>
       </c>
       <c r="R13" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8" t="str">
@@ -8108,16 +8104,16 @@
         <v>9</v>
       </c>
       <c r="L14" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="Q14">
         <v>9</v>
       </c>
       <c r="R14" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8" t="str">
@@ -8129,16 +8125,16 @@
         <v>10</v>
       </c>
       <c r="L15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="Q15">
         <v>10</v>
       </c>
       <c r="R15" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8" t="str">
@@ -8150,16 +8146,16 @@
         <v>11</v>
       </c>
       <c r="L16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="Q16">
         <v>11</v>
       </c>
       <c r="R16" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="8" t="str">
@@ -8171,10 +8167,10 @@
         <v>12</v>
       </c>
       <c r="R17" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="8" t="str">
@@ -8185,10 +8181,10 @@
         <v>13</v>
       </c>
       <c r="R18" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="8" t="str">
@@ -8199,10 +8195,10 @@
         <v>14</v>
       </c>
       <c r="R19" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A20" s="7"/>
       <c r="C20" s="8" t="str">
         <f>Regions!R3</f>
@@ -8212,10 +8208,10 @@
         <v>15</v>
       </c>
       <c r="R20" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A21" s="7"/>
       <c r="C21" s="8" t="str">
         <f>Regions!S3</f>
@@ -8225,10 +8221,10 @@
         <v>16</v>
       </c>
       <c r="R21" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A22" s="7"/>
       <c r="C22" s="8" t="str">
         <f>Regions!T3</f>
@@ -8238,10 +8234,10 @@
         <v>17</v>
       </c>
       <c r="R22" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A23" s="7"/>
       <c r="C23" s="8" t="str">
         <f>Regions!U3</f>
@@ -8251,10 +8247,10 @@
         <v>18</v>
       </c>
       <c r="R23" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A24" s="7"/>
       <c r="C24" s="8" t="str">
         <f>Regions!V3</f>
@@ -8264,10 +8260,10 @@
         <v>19</v>
       </c>
       <c r="R24" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A25" s="7"/>
       <c r="C25" s="8" t="str">
         <f>Regions!W3</f>
@@ -8277,10 +8273,10 @@
         <v>20</v>
       </c>
       <c r="R25" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A26" s="7"/>
       <c r="C26" s="8" t="str">
         <f>Regions!X3</f>
@@ -8290,10 +8286,10 @@
         <v>21</v>
       </c>
       <c r="R26" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A27" s="7"/>
       <c r="C27" s="8" t="str">
         <f>Regions!Y3</f>
@@ -8303,10 +8299,10 @@
         <v>22</v>
       </c>
       <c r="R27" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A28" s="7"/>
       <c r="C28" s="8" t="str">
         <f>Regions!Z3</f>
@@ -8316,41 +8312,41 @@
         <v>23</v>
       </c>
       <c r="R28" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A29" s="7"/>
       <c r="C29" s="8" t="str">
         <f>Regions!AA3</f>
         <v>IE-SO</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A30" s="7"/>
       <c r="C30" s="8" t="str">
         <f>Regions!AB3</f>
         <v>IE-CN</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A31" s="7"/>
       <c r="C31" s="8" t="str">
         <f>Regions!AC3</f>
         <v>IE-DL</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A32" s="7"/>
       <c r="C32" s="8" t="str">
         <f>Regions!AD3</f>
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:28" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A33" s="7"/>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:28" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A34" s="7"/>
       <c r="W34" s="8"/>
       <c r="X34" s="8"/>
@@ -8359,19 +8355,19 @@
       <c r="AA34" s="8"/>
       <c r="AB34" s="8"/>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:28" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A35" s="7"/>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:28" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A36" s="7"/>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:28" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A37" s="7"/>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:28" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A38" s="7"/>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:28" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A39" s="7"/>
     </row>
   </sheetData>
@@ -8395,69 +8391,69 @@
       <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="10" width="13.7109375" customWidth="1"/>
+    <col min="2" max="10" width="13.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:10" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B3" s="12" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="12"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>2018</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:10" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B7" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="12"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:10" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B11" s="12" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="12"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:10" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B12" s="14" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>63</v>
       </c>
       <c r="E12" s="41" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F12" s="14" t="s">
         <v>41</v>
       </c>
       <c r="G12" s="41" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H12" s="41" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="I12" s="41" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J12" s="41" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B13" s="13">
         <v>1</v>
       </c>
@@ -8486,7 +8482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B14" s="13">
         <v>1</v>
       </c>
@@ -8515,7 +8511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B15" s="13">
         <v>1</v>
       </c>
@@ -8544,7 +8540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B16" s="13">
         <v>20</v>
       </c>
@@ -8573,7 +8569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B17" s="13">
         <v>20</v>
       </c>
@@ -8602,7 +8598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.35">
       <c r="C18" s="13">
         <v>5</v>
       </c>
@@ -8628,7 +8624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.35">
       <c r="C19" s="13">
         <v>45</v>
       </c>
@@ -8654,7 +8650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
       <c r="C20" s="13">
         <v>25</v>
       </c>
@@ -8680,7 +8676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.35">
       <c r="C21" s="13">
         <v>5</v>
       </c>
@@ -8706,7 +8702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.35">
       <c r="D22" s="13">
         <v>5</v>
       </c>
@@ -8729,7 +8725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.35">
       <c r="D23" s="13">
         <v>5</v>
       </c>
@@ -8752,7 +8748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.35">
       <c r="D24" s="13">
         <v>5</v>
       </c>
@@ -8775,7 +8771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.35">
       <c r="E25" s="13">
         <v>5</v>
       </c>
@@ -8795,7 +8791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.35">
       <c r="F26" s="13">
         <v>5</v>
       </c>
@@ -8812,7 +8808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.35">
       <c r="F27" s="13">
         <v>5</v>
       </c>
@@ -8829,7 +8825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.35">
       <c r="G28" s="13">
         <v>5</v>
       </c>
@@ -8843,7 +8839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.35">
       <c r="G29" s="13">
         <v>5</v>
       </c>
@@ -8857,7 +8853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.35">
       <c r="G30" s="13">
         <v>5</v>
       </c>
@@ -8871,7 +8867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.35">
       <c r="G31" s="13">
         <v>5</v>
       </c>
@@ -8885,7 +8881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.35">
       <c r="G32" s="13">
         <v>5</v>
       </c>
@@ -8899,7 +8895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="7:10" x14ac:dyDescent="0.35">
       <c r="G33" s="13">
         <v>5</v>
       </c>
@@ -8913,7 +8909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="7:10" x14ac:dyDescent="0.35">
       <c r="G34" s="13">
         <v>5</v>
       </c>
@@ -8927,7 +8923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="7:10" x14ac:dyDescent="0.35">
       <c r="H35" s="13">
         <v>5</v>
       </c>
@@ -8938,7 +8934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="7:10" x14ac:dyDescent="0.35">
       <c r="I36" s="18">
         <v>1</v>
       </c>
@@ -8946,7 +8942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="7:10" x14ac:dyDescent="0.35">
       <c r="I37" s="18">
         <v>1</v>
       </c>
@@ -8954,7 +8950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="7:10" x14ac:dyDescent="0.35">
       <c r="I38" s="18">
         <v>1</v>
       </c>
@@ -8962,7 +8958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="7:10" x14ac:dyDescent="0.35">
       <c r="I39" s="18">
         <v>1</v>
       </c>
@@ -8970,7 +8966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="7:10" x14ac:dyDescent="0.35">
       <c r="I40" s="18">
         <v>1</v>
       </c>
@@ -8978,7 +8974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="7:10" x14ac:dyDescent="0.35">
       <c r="I41" s="18">
         <v>1</v>
       </c>
@@ -8986,7 +8982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="7:10" x14ac:dyDescent="0.35">
       <c r="I42" s="18">
         <v>1</v>
       </c>
@@ -8994,7 +8990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="7:10" x14ac:dyDescent="0.35">
       <c r="I43" s="18">
         <v>1</v>
       </c>
@@ -9002,7 +8998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="7:10" x14ac:dyDescent="0.35">
       <c r="I44" s="18">
         <v>1</v>
       </c>
@@ -9010,7 +9006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="7:10" x14ac:dyDescent="0.35">
       <c r="I45" s="18">
         <v>1</v>
       </c>
@@ -9018,32 +9014,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="7:10" x14ac:dyDescent="0.35">
       <c r="J46" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="7:10" x14ac:dyDescent="0.35">
       <c r="J47" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="7:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="7:10" x14ac:dyDescent="0.35">
       <c r="J48" s="18">
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="10:10" x14ac:dyDescent="0.35">
       <c r="J49" s="18">
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="10:10" x14ac:dyDescent="0.35">
       <c r="J50" s="18">
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="10:10" x14ac:dyDescent="0.35">
       <c r="J51" s="18">
         <v>5</v>
       </c>
@@ -9064,17 +9060,17 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="52.7109375" customWidth="1"/>
+    <col min="2" max="2" width="52.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:3" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B3" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:3" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B4" s="16" t="s">
         <v>29</v>
       </c>
@@ -9082,7 +9078,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B5" s="18" t="s">
         <v>31</v>
       </c>
@@ -9090,7 +9086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B6" s="13" t="s">
         <v>32</v>
       </c>
@@ -9098,7 +9094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B7" s="13" t="s">
         <v>33</v>
       </c>
@@ -9106,7 +9102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B8" s="13" t="s">
         <v>34</v>
       </c>
@@ -9114,7 +9110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B9" s="13" t="s">
         <v>53</v>
       </c>
@@ -9138,42 +9134,42 @@
       <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
-    <col min="7" max="7" width="6.42578125" customWidth="1"/>
-    <col min="8" max="8" width="6.28515625" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.1328125" customWidth="1"/>
+    <col min="6" max="6" width="10.73046875" customWidth="1"/>
+    <col min="7" max="7" width="6.3984375" customWidth="1"/>
+    <col min="8" max="8" width="6.265625" customWidth="1"/>
+    <col min="12" max="12" width="9.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="23"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
       <c r="O2" s="7"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
       <c r="O3" s="25"/>
       <c r="P3" s="25"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
       <c r="O4" s="25"/>
       <c r="P4" s="25"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
       <c r="O5" s="25"/>
       <c r="P5" s="25"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
       <c r="O6" s="25"/>
       <c r="P6" s="25"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
       <c r="O7" s="25"/>
       <c r="P7" s="25"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A8" s="25"/>
       <c r="B8" s="25"/>
       <c r="C8" s="25"/>
@@ -9191,7 +9187,7 @@
       <c r="O8" s="25"/>
       <c r="P8" s="25"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A9" s="25"/>
       <c r="B9" s="25"/>
       <c r="C9" s="25"/>
@@ -9209,7 +9205,7 @@
       <c r="O9" s="25"/>
       <c r="P9" s="25"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A10" s="25"/>
       <c r="B10" s="25"/>
       <c r="C10" s="25"/>
@@ -9227,7 +9223,7 @@
       <c r="O10" s="25"/>
       <c r="P10" s="25"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A11" s="25"/>
       <c r="B11" s="25"/>
       <c r="C11" s="25"/>
@@ -9245,7 +9241,7 @@
       <c r="O11" s="25"/>
       <c r="P11" s="25"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A12" s="25"/>
       <c r="B12" s="25"/>
       <c r="C12" s="25"/>
@@ -9263,7 +9259,7 @@
       <c r="O12" s="25"/>
       <c r="P12" s="25"/>
     </row>
-    <row r="13" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="19" t="s">
         <v>56</v>
       </c>
@@ -9282,7 +9278,7 @@
       <c r="O13" s="25"/>
       <c r="P13" s="25"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A14" s="24" t="s">
         <v>0</v>
       </c>
@@ -9302,7 +9298,7 @@
       <c r="O14" s="25"/>
       <c r="P14" s="25"/>
     </row>
-    <row r="15" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="21" t="s">
         <v>16</v>
       </c>
@@ -9352,7 +9348,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A16" s="25"/>
       <c r="B16" s="25"/>
       <c r="C16" s="25" t="s">
@@ -9378,7 +9374,7 @@
       <c r="O16" s="25"/>
       <c r="P16" s="25"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A17" s="25"/>
       <c r="B17" s="25"/>
       <c r="C17" s="25" t="s">
@@ -9404,7 +9400,7 @@
       <c r="O17" s="25"/>
       <c r="P17" s="25"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A18" s="25"/>
       <c r="B18" s="25"/>
       <c r="C18" s="25"/>
@@ -9422,7 +9418,7 @@
       <c r="O18" s="25"/>
       <c r="P18" s="25"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A19" s="25"/>
       <c r="B19" s="25"/>
       <c r="C19" s="25"/>
@@ -9440,7 +9436,7 @@
       <c r="O19" s="25"/>
       <c r="P19" s="25"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A20" s="25"/>
       <c r="B20" s="25"/>
       <c r="C20" s="25"/>
@@ -9458,7 +9454,7 @@
       <c r="O20" s="25"/>
       <c r="P20" s="25"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A21" s="25"/>
       <c r="B21" s="25"/>
       <c r="C21" s="25"/>
@@ -9476,7 +9472,7 @@
       <c r="O21" s="25"/>
       <c r="P21" s="25"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A22" s="25"/>
       <c r="B22" s="25"/>
       <c r="C22" s="25"/>
@@ -9494,7 +9490,7 @@
       <c r="O22" s="25"/>
       <c r="P22" s="25"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A23" s="25"/>
       <c r="B23" s="25"/>
       <c r="C23" s="25"/>
@@ -9512,7 +9508,7 @@
       <c r="O23" s="25"/>
       <c r="P23" s="25"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A24" s="25"/>
       <c r="B24" s="25"/>
       <c r="C24" s="25"/>
@@ -9542,31 +9538,31 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="B1:G34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.1328125" customWidth="1"/>
+    <col min="3" max="3" width="10.86328125" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="5" max="5" width="6.1328125" customWidth="1"/>
+    <col min="6" max="6" width="17.59765625" customWidth="1"/>
+    <col min="7" max="7" width="10.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B1" s="23" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B3" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="9" t="s">
         <v>16</v>
       </c>
@@ -9586,7 +9582,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
       <c r="D5" s="7" t="s">
         <v>43</v>
       </c>
@@ -9594,7 +9590,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B6" s="27"/>
       <c r="C6" s="27"/>
       <c r="D6" s="27" t="s">
@@ -9606,373 +9602,375 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B7" s="27"/>
       <c r="C7" s="27" t="str">
-        <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B3,2))</f>
-        <v>EUR00</v>
+        <f>_xlfn.CONCAT("MEUR",RIGHT(CPI!B3,4))</f>
+        <v>MEUR2000</v>
       </c>
       <c r="D7" s="27" t="s">
         <v>45</v>
       </c>
       <c r="E7" s="27"/>
       <c r="F7" s="27" t="s">
-        <v>64</v>
+        <v>172</v>
       </c>
       <c r="G7" s="28">
         <f>CPI!$D$21/CPI!D3</f>
         <v>1.3926669328933141</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B8" s="7"/>
       <c r="C8" s="7" t="str">
-        <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B4,2))</f>
-        <v>EUR01</v>
+        <f>_xlfn.CONCAT("MEUR",RIGHT(CPI!B4,4))</f>
+        <v>MEUR2001</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>45</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7" t="s">
-        <v>64</v>
+        <v>172</v>
       </c>
       <c r="G8" s="26">
         <f>CPI!$D$21/CPI!D4</f>
         <v>1.3626878012654737</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B9" s="7"/>
       <c r="C9" s="7" t="str">
-        <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B5,2))</f>
-        <v>EUR02</v>
+        <f>_xlfn.CONCAT("MEUR",RIGHT(CPI!B5,4))</f>
+        <v>MEUR2002</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>45</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7" t="s">
-        <v>64</v>
+        <v>172</v>
       </c>
       <c r="G9" s="26">
         <f>CPI!$D$21/CPI!D5</f>
         <v>1.3346599424735295</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B10" s="7"/>
       <c r="C10" s="7" t="str">
-        <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B6,2))</f>
-        <v>EUR03</v>
+        <f>_xlfn.CONCAT("MEUR",RIGHT(CPI!B6,4))</f>
+        <v>MEUR2003</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>45</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7" t="s">
-        <v>64</v>
+        <v>172</v>
       </c>
       <c r="G10" s="26">
         <f>CPI!$D$21/CPI!D6</f>
         <v>1.3084901396799309</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B11" s="7"/>
       <c r="C11" s="7" t="str">
-        <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B7,2))</f>
-        <v>EUR04</v>
+        <f>_xlfn.CONCAT("MEUR",RIGHT(CPI!B7,4))</f>
+        <v>MEUR2004</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>45</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7" t="s">
-        <v>64</v>
+        <v>172</v>
       </c>
       <c r="G11" s="26">
         <f>CPI!$D$21/CPI!D7</f>
         <v>1.2828334702744419</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B12" s="7"/>
       <c r="C12" s="7" t="str">
-        <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B8,2))</f>
-        <v>EUR05</v>
+        <f>_xlfn.CONCAT("MEUR",RIGHT(CPI!B8,4))</f>
+        <v>MEUR2005</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>45</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7" t="s">
-        <v>64</v>
+        <v>172</v>
       </c>
       <c r="G12" s="26">
         <f>CPI!$D$21/CPI!D8</f>
         <v>1.2552186597597279</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B13" s="7"/>
       <c r="C13" s="7" t="str">
-        <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B9,2))</f>
-        <v>EUR06</v>
+        <f>_xlfn.CONCAT("MEUR",RIGHT(CPI!B9,4))</f>
+        <v>MEUR2006</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>45</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7" t="s">
-        <v>64</v>
+        <v>172</v>
       </c>
       <c r="G13" s="26">
         <f>CPI!$D$21/CPI!D9</f>
         <v>1.2281982972208687</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B14" s="7"/>
       <c r="C14" s="7" t="str">
-        <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B10,2))</f>
-        <v>EUR07</v>
+        <f>_xlfn.CONCAT("MEUR",RIGHT(CPI!B10,4))</f>
+        <v>MEUR2007</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>45</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7" t="s">
-        <v>64</v>
+        <v>172</v>
       </c>
       <c r="G14" s="26">
         <f>CPI!$D$21/CPI!D10</f>
         <v>1.2005848457682002</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B15" s="7"/>
       <c r="C15" s="7" t="str">
-        <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B11,2))</f>
-        <v>EUR08</v>
+        <f>_xlfn.CONCAT("MEUR",RIGHT(CPI!B11,4))</f>
+        <v>MEUR2008</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>45</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7" t="s">
-        <v>64</v>
+        <v>172</v>
       </c>
       <c r="G15" s="26">
         <f>CPI!$D$21/CPI!D11</f>
         <v>1.1577481637108971</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B16" s="7"/>
       <c r="C16" s="7" t="str">
-        <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B12,2))</f>
-        <v>EUR09</v>
+        <f>_xlfn.CONCAT("MEUR",RIGHT(CPI!B12,4))</f>
+        <v>MEUR2009</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>45</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7" t="s">
-        <v>64</v>
+        <v>172</v>
       </c>
       <c r="G16" s="26">
         <f>CPI!$D$21/CPI!D12</f>
         <v>1.1462853106048485</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B17" s="7"/>
       <c r="C17" s="7" t="str">
-        <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B13,2))</f>
-        <v>EUR10</v>
+        <f>_xlfn.CONCAT("MEUR",RIGHT(CPI!B13,4))</f>
+        <v>MEUR2010</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>45</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7" t="s">
-        <v>64</v>
+        <v>172</v>
       </c>
       <c r="G17" s="26">
         <f>CPI!$D$21/CPI!D13</f>
         <v>1.1227084335013209</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B18" s="7"/>
       <c r="C18" s="7" t="str">
-        <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B14,2))</f>
-        <v>EUR11</v>
+        <f>_xlfn.CONCAT("MEUR",RIGHT(CPI!B14,4))</f>
+        <v>MEUR2011</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>45</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7" t="s">
-        <v>64</v>
+        <v>172</v>
       </c>
       <c r="G18" s="26">
         <f>CPI!$D$21/CPI!D14</f>
         <v>1.0889509539295061</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B19" s="7"/>
       <c r="C19" s="7" t="str">
-        <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B15,2))</f>
-        <v>EUR12</v>
+        <f>_xlfn.CONCAT("MEUR",RIGHT(CPI!B15,4))</f>
+        <v>MEUR2012</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>45</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7" t="s">
-        <v>64</v>
+        <v>172</v>
       </c>
       <c r="G19" s="26">
         <f>CPI!$D$21/CPI!D15</f>
         <v>1.0613557055843141</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B20" s="7"/>
       <c r="C20" s="7" t="str">
-        <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B16,2))</f>
-        <v>EUR13</v>
+        <f>_xlfn.CONCAT("MEUR",RIGHT(CPI!B16,4))</f>
+        <v>MEUR2013</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>45</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7" t="s">
-        <v>64</v>
+        <v>172</v>
       </c>
       <c r="G20" s="26">
         <f>CPI!$D$21/CPI!D16</f>
         <v>1.045670645895876</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B21" s="7"/>
       <c r="C21" s="7" t="str">
-        <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B17,2))</f>
-        <v>EUR14</v>
+        <f>_xlfn.CONCAT("MEUR",RIGHT(CPI!B17,4))</f>
+        <v>MEUR2014</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>45</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7" t="s">
-        <v>64</v>
+        <v>172</v>
       </c>
       <c r="G21" s="26">
         <f>CPI!$D$21/CPI!D17</f>
         <v>1.0394340416460002</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B22" s="7"/>
       <c r="C22" s="7" t="str">
-        <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B18,2))</f>
-        <v>EUR15</v>
+        <f>_xlfn.CONCAT("MEUR",RIGHT(CPI!B18,4))</f>
+        <v>MEUR2015</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>45</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7" t="s">
-        <v>64</v>
+        <v>172</v>
       </c>
       <c r="G22" s="26">
         <f>CPI!$D$21/CPI!D18</f>
         <v>1.0383956459999999</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B23" s="7"/>
       <c r="C23" s="7" t="str">
-        <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B19,2))</f>
-        <v>EUR16</v>
+        <f>_xlfn.CONCAT("MEUR",RIGHT(CPI!B19,4))</f>
+        <v>MEUR2016</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>45</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7" t="s">
-        <v>64</v>
+        <v>172</v>
       </c>
       <c r="G23" s="26">
         <f>CPI!$D$21/CPI!D19</f>
         <v>1.0363230000000001</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B24" s="7"/>
       <c r="C24" s="7" t="str">
-        <f>_xlfn.CONCAT("EUR",RIGHT(CPI!B20,2))</f>
-        <v>EUR17</v>
+        <f>_xlfn.CONCAT("MEUR",RIGHT(CPI!B20,4))</f>
+        <v>MEUR2017</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>45</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="7" t="s">
-        <v>64</v>
+        <v>172</v>
       </c>
       <c r="G24" s="26">
         <f>CPI!$D$21/CPI!D20</f>
         <v>1.0190000000000001</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B25" s="7"/>
-      <c r="C25" s="7" t="s">
-        <v>65</v>
+      <c r="C25" s="7" t="str">
+        <f>_xlfn.CONCAT("MEUR",RIGHT(CPI!B22,4))</f>
+        <v>MEUR2019</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>45</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7" t="s">
-        <v>64</v>
+        <v>172</v>
       </c>
       <c r="G25" s="26">
         <f>CPI!$D$21/CPI!D22</f>
         <v>0.98522167487684731</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C26" s="7" t="s">
-        <v>153</v>
+    <row r="26" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
+      <c r="C26" s="7" t="str">
+        <f>_xlfn.CONCAT("MEUR",RIGHT(CPI!B23,4))</f>
+        <v>MEUR2020</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>45</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7" t="s">
-        <v>64</v>
+        <v>172</v>
       </c>
       <c r="G26" s="26">
         <f>CPI!$D$21/CPI!D23</f>
         <v>0.9783730634328176</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B31" s="7"/>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B32" s="7"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:2" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B33" s="7"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:2" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B34" s="26"/>
     </row>
   </sheetData>
@@ -9988,26 +9986,26 @@
   <dimension ref="B2:O24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:15" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B2" s="11" t="s">
         <v>47</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M2" s="11" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="3" spans="2:15" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B3" s="9" t="s">
         <v>48</v>
       </c>
@@ -10024,30 +10022,30 @@
         <v>59</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>49</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="K3" s="9" t="s">
         <v>60</v>
       </c>
       <c r="M3" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="O3" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="N3" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="O3" s="9" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="2:15" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B4" s="7" t="s">
-        <v>64</v>
+        <v>172</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>50</v>
@@ -10065,7 +10063,7 @@
         <v>61</v>
       </c>
       <c r="M4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="N4" t="s">
         <v>61</v>
@@ -10074,19 +10072,19 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:15" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B5" s="7" t="str">
         <f>Constants!C7</f>
-        <v>EUR00</v>
+        <v>MEUR2000</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>62</v>
@@ -10095,19 +10093,19 @@
         <v>62</v>
       </c>
       <c r="M5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="N5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="O5">
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:15" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B6" s="7" t="str">
         <f>Constants!C8</f>
-        <v>EUR01</v>
+        <v>MEUR2001</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>52</v>
@@ -10125,22 +10123,22 @@
         <v>61</v>
       </c>
       <c r="M6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="N6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="O6">
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:15" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B7" s="7" t="str">
         <f>Constants!C9</f>
-        <v>EUR02</v>
+        <v>MEUR2002</v>
       </c>
       <c r="M7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="N7" t="s">
         <v>61</v>
@@ -10149,13 +10147,13 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:15" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B8" s="7" t="str">
         <f>Constants!C10</f>
-        <v>EUR03</v>
+        <v>MEUR2003</v>
       </c>
       <c r="M8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="N8" t="s">
         <v>61</v>
@@ -10164,13 +10162,13 @@
         <v>41.87</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:15" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B9" s="7" t="str">
         <f>Constants!C11</f>
-        <v>EUR04</v>
+        <v>MEUR2004</v>
       </c>
       <c r="M9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="N9" t="s">
         <v>61</v>
@@ -10179,28 +10177,28 @@
         <v>3.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:15" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B10" s="7" t="str">
         <f>Constants!C12</f>
-        <v>EUR05</v>
+        <v>MEUR2005</v>
       </c>
       <c r="M10" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="N10" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="O10">
         <v>1000000</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:15" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B11" s="7" t="str">
         <f>Constants!C13</f>
-        <v>EUR06</v>
+        <v>MEUR2006</v>
       </c>
       <c r="M11" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="N11" t="s">
         <v>61</v>
@@ -10209,13 +10207,13 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:15" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B12" s="7" t="str">
         <f>Constants!C14</f>
-        <v>EUR07</v>
+        <v>MEUR2007</v>
       </c>
       <c r="M12" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="N12" t="s">
         <v>61</v>
@@ -10224,10 +10222,10 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:15" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B13" s="7" t="str">
         <f>Constants!C15</f>
-        <v>EUR08</v>
+        <v>MEUR2008</v>
       </c>
       <c r="M13" t="s">
         <v>61</v>
@@ -10239,88 +10237,88 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:15" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B14" s="7" t="str">
         <f>Constants!C16</f>
-        <v>EUR09</v>
+        <v>MEUR2009</v>
       </c>
       <c r="M14" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="N14" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="O14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:15" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B15" s="7" t="str">
         <f>Constants!C17</f>
-        <v>EUR10</v>
+        <v>MEUR2010</v>
       </c>
       <c r="M15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="N15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="O15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:15" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B16" s="7" t="str">
         <f>Constants!C18</f>
-        <v>EUR11</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+        <v>MEUR2011</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B17" s="7" t="str">
         <f>Constants!C19</f>
-        <v>EUR12</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+        <v>MEUR2012</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B18" s="7" t="str">
         <f>Constants!C20</f>
-        <v>EUR13</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+        <v>MEUR2013</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B19" s="7" t="str">
         <f>Constants!C21</f>
-        <v>EUR14</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+        <v>MEUR2014</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B20" s="7" t="str">
         <f>Constants!C22</f>
-        <v>EUR15</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+        <v>MEUR2015</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B21" s="7" t="str">
         <f>Constants!C23</f>
-        <v>EUR16</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+        <v>MEUR2016</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B22" s="7" t="str">
         <f>Constants!C24</f>
-        <v>EUR17</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+        <v>MEUR2017</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B23" s="7" t="str">
         <f>Constants!C25</f>
-        <v>EUR19</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
+        <v>MEUR2019</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B24" s="7" t="str">
         <f>Constants!C26</f>
-        <v>EUR20</v>
+        <v>MEUR2020</v>
       </c>
     </row>
   </sheetData>
@@ -10339,13 +10337,13 @@
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="4" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.3984375" customWidth="1"/>
+    <col min="3" max="4" width="13.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="29"/>
       <c r="C2" s="30" t="s">
         <v>38</v>
@@ -10354,7 +10352,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
       <c r="B3" s="32">
         <v>2000</v>
       </c>
@@ -10363,7 +10361,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
       <c r="B4" s="32">
         <v>2001</v>
       </c>
@@ -10375,7 +10373,7 @@
         <v>102.2</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
       <c r="B5" s="32">
         <v>2002</v>
       </c>
@@ -10387,7 +10385,7 @@
         <v>104.34620000000001</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
       <c r="B6" s="32">
         <v>2003</v>
       </c>
@@ -10399,7 +10397,7 @@
         <v>106.43312400000001</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
       <c r="B7" s="32">
         <v>2004</v>
       </c>
@@ -10411,7 +10409,7 @@
         <v>108.56178648000001</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
       <c r="B8" s="32">
         <v>2005</v>
       </c>
@@ -10423,7 +10421,7 @@
         <v>110.95014578256001</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
       <c r="B9" s="32">
         <v>2006</v>
       </c>
@@ -10435,7 +10433,7 @@
         <v>113.39104898977634</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
       <c r="B10" s="32">
         <v>2007</v>
       </c>
@@ -10447,7 +10445,7 @@
         <v>115.99904311654119</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
       <c r="B11" s="32">
         <v>2008</v>
       </c>
@@ -10459,7 +10457,7 @@
         <v>120.29100771185321</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
       <c r="B12" s="32">
         <v>2009</v>
       </c>
@@ -10471,7 +10469,7 @@
         <v>121.49391778897174</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
       <c r="B13" s="32">
         <v>2010</v>
       </c>
@@ -10483,7 +10481,7 @@
         <v>124.04529006254015</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
       <c r="B14" s="32">
         <v>2011</v>
       </c>
@@ -10495,7 +10493,7 @@
         <v>127.89069405447889</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
       <c r="B15" s="32">
         <v>2012</v>
       </c>
@@ -10507,7 +10505,7 @@
         <v>131.21585209989533</v>
       </c>
     </row>
-    <row r="16" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
       <c r="B16" s="32">
         <v>2013</v>
       </c>
@@ -10519,7 +10517,7 @@
         <v>133.18408988139376</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
       <c r="B17" s="32">
         <v>2014</v>
       </c>
@@ -10531,7 +10529,7 @@
         <v>133.98319442068211</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
       <c r="B18" s="32">
         <v>2015</v>
       </c>
@@ -10543,7 +10541,7 @@
         <v>134.1171776151028</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
       <c r="B19" s="37">
         <v>2016</v>
       </c>
@@ -10555,7 +10553,7 @@
         <v>134.385411970333</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
       <c r="B20" s="37">
         <v>2017</v>
       </c>
@@ -10567,7 +10565,7 @@
         <v>136.66996397382866</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
       <c r="B21" s="37">
         <v>2018</v>
       </c>
@@ -10579,7 +10577,7 @@
         <v>139.26669328933141</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
       <c r="B22" s="37">
         <v>2019</v>
       </c>
@@ -10591,7 +10589,7 @@
         <v>141.35569368867138</v>
       </c>
     </row>
-    <row r="23" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
       <c r="B23" s="37">
         <v>2020</v>
       </c>
@@ -10603,7 +10601,7 @@
         <v>142.34518354449207</v>
       </c>
     </row>
-    <row r="25" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:4" ht="14.25" x14ac:dyDescent="0.35">
       <c r="B25" s="36" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
Delete P22 to avoid model infeasibility and use P23 as default instead
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{273CD800-4683-4C80-89EA-6D14D4E26CE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D6EC06-CAFD-4669-8E22-3A4E307F0B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="28" r:id="rId1"/>
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="162">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -549,9 +549,6 @@
   </si>
   <si>
     <t>P9</t>
-  </si>
-  <si>
-    <t>P22</t>
   </si>
   <si>
     <t>P23</t>
@@ -2271,7 +2268,7 @@
       <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>2859</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
@@ -4462,7 +4459,7 @@
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="57" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B16" s="57"/>
       <c r="C16" s="57"/>
@@ -4548,10 +4545,10 @@
     </row>
     <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="48" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B19" s="56" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C19" s="56"/>
       <c r="D19" s="56"/>
@@ -4580,10 +4577,10 @@
     </row>
     <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="48" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B20" s="56" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C20" s="56"/>
       <c r="D20" s="56"/>
@@ -4612,10 +4609,10 @@
     </row>
     <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="48" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B21" s="51" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C21" s="51"/>
       <c r="D21" s="51"/>
@@ -4672,10 +4669,10 @@
     </row>
     <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="48" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B23" s="56" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C23" s="56"/>
       <c r="D23" s="56"/>
@@ -4760,10 +4757,10 @@
     </row>
     <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="48" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B26" s="56" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C26" s="56"/>
       <c r="D26" s="56"/>
@@ -4848,7 +4845,7 @@
     </row>
     <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="48" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B29" s="52">
         <v>1</v>
@@ -4880,10 +4877,10 @@
     </row>
     <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="48" t="s">
+        <v>151</v>
+      </c>
+      <c r="B30" s="58" t="s">
         <v>152</v>
-      </c>
-      <c r="B30" s="58" t="s">
-        <v>153</v>
       </c>
       <c r="C30" s="56"/>
       <c r="D30" s="56"/>
@@ -4912,10 +4909,10 @@
     </row>
     <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="B31" s="56" t="s">
         <v>154</v>
-      </c>
-      <c r="B31" s="56" t="s">
-        <v>155</v>
       </c>
       <c r="C31" s="56"/>
       <c r="D31" s="56"/>
@@ -4945,7 +4942,7 @@
     <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="54"/>
       <c r="B32" s="55" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C32" s="54"/>
       <c r="D32" s="54"/>
@@ -7555,8 +7552,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A3:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W12" sqref="W12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7825,46 +7822,46 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="B3:J51"/>
+  <dimension ref="B3:I51"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="10" width="13.7109375" customWidth="1"/>
+    <col min="2" max="9" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B3" s="11" t="s">
         <v>31</v>
       </c>
       <c r="C3" s="11"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>2018</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B7" s="11" t="s">
         <v>32</v>
       </c>
       <c r="C7" s="11"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B11" s="11" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="11"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B12" s="13" t="s">
         <v>137</v>
       </c>
@@ -7884,16 +7881,13 @@
         <v>139</v>
       </c>
       <c r="H12" s="39" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="I12" s="39" t="s">
-        <v>135</v>
-      </c>
-      <c r="J12" s="39" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" s="12">
         <v>1</v>
       </c>
@@ -7910,19 +7904,16 @@
         <v>1</v>
       </c>
       <c r="G13" s="12">
-        <v>2</v>
-      </c>
-      <c r="H13" s="12">
+        <v>1</v>
+      </c>
+      <c r="H13" s="17">
         <v>1</v>
       </c>
       <c r="I13" s="17">
         <v>1</v>
       </c>
-      <c r="J13" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B14" s="12">
         <v>1</v>
       </c>
@@ -7941,17 +7932,14 @@
       <c r="G14" s="12">
         <v>1</v>
       </c>
-      <c r="H14" s="12">
+      <c r="H14" s="17">
         <v>1</v>
       </c>
       <c r="I14" s="17">
         <v>1</v>
       </c>
-      <c r="J14" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B15" s="12">
         <v>1</v>
       </c>
@@ -7970,17 +7958,14 @@
       <c r="G15" s="12">
         <v>1</v>
       </c>
-      <c r="H15" s="12">
+      <c r="H15" s="17">
         <v>1</v>
       </c>
       <c r="I15" s="17">
         <v>1</v>
       </c>
-      <c r="J15" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B16" s="12">
         <v>20</v>
       </c>
@@ -7999,17 +7984,14 @@
       <c r="G16" s="12">
         <v>1</v>
       </c>
-      <c r="H16" s="12">
+      <c r="H16" s="17">
         <v>1</v>
       </c>
       <c r="I16" s="17">
         <v>1</v>
       </c>
-      <c r="J16" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" s="12">
         <v>20</v>
       </c>
@@ -8028,17 +8010,14 @@
       <c r="G17" s="12">
         <v>1</v>
       </c>
-      <c r="H17" s="12">
+      <c r="H17" s="17">
         <v>1</v>
       </c>
       <c r="I17" s="17">
         <v>1</v>
       </c>
-      <c r="J17" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C18" s="12">
         <v>5</v>
       </c>
@@ -8054,17 +8033,14 @@
       <c r="G18" s="12">
         <v>1</v>
       </c>
-      <c r="H18" s="12">
+      <c r="H18" s="17">
         <v>1</v>
       </c>
       <c r="I18" s="17">
         <v>1</v>
       </c>
-      <c r="J18" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C19" s="12">
         <v>45</v>
       </c>
@@ -8080,17 +8056,14 @@
       <c r="G19" s="12">
         <v>1</v>
       </c>
-      <c r="H19" s="12">
+      <c r="H19" s="17">
         <v>1</v>
       </c>
       <c r="I19" s="17">
         <v>1</v>
       </c>
-      <c r="J19" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C20" s="12">
         <v>25</v>
       </c>
@@ -8106,17 +8079,14 @@
       <c r="G20" s="12">
         <v>1</v>
       </c>
-      <c r="H20" s="12">
+      <c r="H20" s="17">
         <v>1</v>
       </c>
       <c r="I20" s="17">
         <v>1</v>
       </c>
-      <c r="J20" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C21" s="12">
         <v>5</v>
       </c>
@@ -8132,17 +8102,14 @@
       <c r="G21" s="12">
         <v>1</v>
       </c>
-      <c r="H21" s="12">
+      <c r="H21" s="17">
         <v>1</v>
       </c>
       <c r="I21" s="17">
         <v>1</v>
       </c>
-      <c r="J21" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D22" s="12">
         <v>5</v>
       </c>
@@ -8155,17 +8122,14 @@
       <c r="G22" s="12">
         <v>1</v>
       </c>
-      <c r="H22" s="12">
+      <c r="H22" s="17">
         <v>1</v>
       </c>
       <c r="I22" s="17">
         <v>1</v>
       </c>
-      <c r="J22" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D23" s="12">
         <v>5</v>
       </c>
@@ -8178,17 +8142,14 @@
       <c r="G23" s="12">
         <v>1</v>
       </c>
-      <c r="H23" s="12">
+      <c r="H23" s="17">
         <v>1</v>
       </c>
       <c r="I23" s="17">
         <v>1</v>
       </c>
-      <c r="J23" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D24" s="12">
         <v>5</v>
       </c>
@@ -8201,17 +8162,14 @@
       <c r="G24" s="12">
         <v>1</v>
       </c>
-      <c r="H24" s="12">
+      <c r="H24" s="17">
         <v>1</v>
       </c>
       <c r="I24" s="17">
         <v>1</v>
       </c>
-      <c r="J24" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="E25" s="12">
         <v>5</v>
       </c>
@@ -8221,266 +8179,236 @@
       <c r="G25" s="12">
         <v>1</v>
       </c>
-      <c r="H25" s="12">
+      <c r="H25" s="17">
         <v>1</v>
       </c>
       <c r="I25" s="17">
         <v>1</v>
       </c>
-      <c r="J25" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="F26" s="12">
         <v>5</v>
       </c>
       <c r="G26" s="12">
         <v>1</v>
       </c>
-      <c r="H26" s="12">
+      <c r="H26" s="17">
         <v>1</v>
       </c>
       <c r="I26" s="17">
         <v>1</v>
       </c>
-      <c r="J26" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
       <c r="F27" s="12">
         <v>5</v>
       </c>
       <c r="G27" s="12">
-        <v>5</v>
-      </c>
-      <c r="H27" s="12">
+        <v>1</v>
+      </c>
+      <c r="H27" s="17">
         <v>1</v>
       </c>
       <c r="I27" s="17">
         <v>1</v>
       </c>
-      <c r="J27" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
       <c r="G28" s="12">
         <v>5</v>
       </c>
-      <c r="H28" s="12">
-        <v>5</v>
+      <c r="H28" s="17">
+        <v>1</v>
       </c>
       <c r="I28" s="17">
         <v>1</v>
       </c>
-      <c r="J28" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
       <c r="G29" s="12">
         <v>5</v>
       </c>
-      <c r="H29" s="12">
-        <v>5</v>
+      <c r="H29" s="17">
+        <v>1</v>
       </c>
       <c r="I29" s="17">
         <v>1</v>
       </c>
-      <c r="J29" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
       <c r="G30" s="12">
         <v>5</v>
       </c>
-      <c r="H30" s="12">
-        <v>5</v>
+      <c r="H30" s="17">
+        <v>1</v>
       </c>
       <c r="I30" s="17">
         <v>1</v>
       </c>
-      <c r="J30" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
       <c r="G31" s="12">
         <v>5</v>
       </c>
-      <c r="H31" s="12">
-        <v>5</v>
+      <c r="H31" s="17">
+        <v>1</v>
       </c>
       <c r="I31" s="17">
         <v>1</v>
       </c>
-      <c r="J31" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
       <c r="G32" s="12">
         <v>5</v>
       </c>
-      <c r="H32" s="12">
-        <v>5</v>
+      <c r="H32" s="17">
+        <v>1</v>
       </c>
       <c r="I32" s="17">
         <v>1</v>
       </c>
-      <c r="J32" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="7:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G33" s="12">
         <v>5</v>
       </c>
-      <c r="H33" s="12">
-        <v>5</v>
+      <c r="H33" s="17">
+        <v>1</v>
       </c>
       <c r="I33" s="17">
         <v>1</v>
       </c>
-      <c r="J33" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="7:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="7:9" x14ac:dyDescent="0.2">
       <c r="G34" s="12">
         <v>5</v>
       </c>
-      <c r="H34" s="12">
+      <c r="H34" s="17">
+        <v>1</v>
+      </c>
+      <c r="I34" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G35" s="12">
         <v>5</v>
       </c>
-      <c r="I34" s="17">
-        <v>1</v>
-      </c>
-      <c r="J34" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="7:10" x14ac:dyDescent="0.2">
-      <c r="H35" s="12">
+      <c r="H35" s="17">
+        <v>1</v>
+      </c>
+      <c r="I35" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="H36" s="17">
+        <v>1</v>
+      </c>
+      <c r="I36" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="H37" s="17">
+        <v>1</v>
+      </c>
+      <c r="I37" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="H38" s="17">
+        <v>1</v>
+      </c>
+      <c r="I38" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="H39" s="17">
+        <v>1</v>
+      </c>
+      <c r="I39" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="H40" s="17">
+        <v>1</v>
+      </c>
+      <c r="I40" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="H41" s="17">
+        <v>1</v>
+      </c>
+      <c r="I41" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="H42" s="17">
+        <v>1</v>
+      </c>
+      <c r="I42" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="H43" s="17">
+        <v>1</v>
+      </c>
+      <c r="I43" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="H44" s="17">
+        <v>1</v>
+      </c>
+      <c r="I44" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="H45" s="17">
+        <v>1</v>
+      </c>
+      <c r="I45" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="I46" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="I47" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="I48" s="17">
         <v>5</v>
       </c>
-      <c r="I35" s="17">
-        <v>1</v>
-      </c>
-      <c r="J35" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="7:10" x14ac:dyDescent="0.2">
-      <c r="I36" s="17">
-        <v>1</v>
-      </c>
-      <c r="J36" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="7:10" x14ac:dyDescent="0.2">
-      <c r="I37" s="17">
-        <v>1</v>
-      </c>
-      <c r="J37" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="7:10" x14ac:dyDescent="0.2">
-      <c r="I38" s="17">
-        <v>1</v>
-      </c>
-      <c r="J38" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="7:10" x14ac:dyDescent="0.2">
-      <c r="I39" s="17">
-        <v>1</v>
-      </c>
-      <c r="J39" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="7:10" x14ac:dyDescent="0.2">
-      <c r="I40" s="17">
-        <v>1</v>
-      </c>
-      <c r="J40" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="7:10" x14ac:dyDescent="0.2">
-      <c r="I41" s="17">
-        <v>1</v>
-      </c>
-      <c r="J41" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="7:10" x14ac:dyDescent="0.2">
-      <c r="I42" s="17">
-        <v>1</v>
-      </c>
-      <c r="J42" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="7:10" x14ac:dyDescent="0.2">
-      <c r="I43" s="17">
-        <v>1</v>
-      </c>
-      <c r="J43" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="7:10" x14ac:dyDescent="0.2">
-      <c r="I44" s="17">
-        <v>1</v>
-      </c>
-      <c r="J44" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="7:10" x14ac:dyDescent="0.2">
-      <c r="I45" s="17">
-        <v>1</v>
-      </c>
-      <c r="J45" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="7:10" x14ac:dyDescent="0.2">
-      <c r="J46" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="7:10" x14ac:dyDescent="0.2">
-      <c r="J47" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="7:10" x14ac:dyDescent="0.2">
-      <c r="J48" s="17">
+    </row>
+    <row r="49" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I49" s="17">
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J49" s="17">
+    <row r="50" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I50" s="17">
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J50" s="17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="51" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J51" s="17">
+    <row r="51" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I51" s="17">
         <v>5</v>
       </c>
     </row>
@@ -9053,7 +8981,7 @@
       </c>
       <c r="E7" s="26"/>
       <c r="F7" s="26" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G7" s="27">
         <f>CPI!$D$21/CPI!D3</f>
@@ -9071,7 +8999,7 @@
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G8" s="25">
         <f>CPI!$D$21/CPI!D4</f>
@@ -9089,7 +9017,7 @@
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G9" s="25">
         <f>CPI!$D$21/CPI!D5</f>
@@ -9107,7 +9035,7 @@
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G10" s="25">
         <f>CPI!$D$21/CPI!D6</f>
@@ -9125,7 +9053,7 @@
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G11" s="25">
         <f>CPI!$D$21/CPI!D7</f>
@@ -9143,7 +9071,7 @@
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G12" s="25">
         <f>CPI!$D$21/CPI!D8</f>
@@ -9161,7 +9089,7 @@
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G13" s="25">
         <f>CPI!$D$21/CPI!D9</f>
@@ -9179,7 +9107,7 @@
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G14" s="25">
         <f>CPI!$D$21/CPI!D10</f>
@@ -9197,7 +9125,7 @@
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G15" s="25">
         <f>CPI!$D$21/CPI!D11</f>
@@ -9215,7 +9143,7 @@
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G16" s="25">
         <f>CPI!$D$21/CPI!D12</f>
@@ -9233,7 +9161,7 @@
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G17" s="25">
         <f>CPI!$D$21/CPI!D13</f>
@@ -9251,7 +9179,7 @@
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G18" s="25">
         <f>CPI!$D$21/CPI!D14</f>
@@ -9269,7 +9197,7 @@
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G19" s="25">
         <f>CPI!$D$21/CPI!D15</f>
@@ -9287,7 +9215,7 @@
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G20" s="25">
         <f>CPI!$D$21/CPI!D16</f>
@@ -9305,7 +9233,7 @@
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G21" s="25">
         <f>CPI!$D$21/CPI!D17</f>
@@ -9323,7 +9251,7 @@
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G22" s="25">
         <f>CPI!$D$21/CPI!D18</f>
@@ -9341,7 +9269,7 @@
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G23" s="25">
         <f>CPI!$D$21/CPI!D19</f>
@@ -9359,7 +9287,7 @@
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G24" s="25">
         <f>CPI!$D$21/CPI!D20</f>
@@ -9377,7 +9305,7 @@
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G25" s="25">
         <f>CPI!$D$21/CPI!D22</f>
@@ -9394,7 +9322,7 @@
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G26" s="25">
         <f>CPI!$D$21/CPI!D23</f>
@@ -9411,7 +9339,7 @@
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G27" s="25">
         <f>CPI!$D$21/CPI!D24</f>
@@ -9479,13 +9407,13 @@
         <v>55</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>45</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K3" s="9" t="s">
         <v>56</v>
@@ -9502,7 +9430,7 @@
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B4" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>46</v>
@@ -9538,10 +9466,10 @@
         <v>47</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
Increase Dummy Price. Check as dummies are created is small amounts after fuel optimisation.
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D6EC06-CAFD-4669-8E22-3A4E307F0B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004912E0-20DC-414D-BED2-579E803A8916}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="28" r:id="rId1"/>
@@ -106,7 +106,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -7824,7 +7823,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B3:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
@@ -8498,8 +8497,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8725,7 +8724,7 @@
       <c r="D16" s="24"/>
       <c r="E16" s="24"/>
       <c r="F16" s="24">
-        <v>2222</v>
+        <v>22222</v>
       </c>
       <c r="G16" s="24"/>
       <c r="H16" s="24"/>
@@ -8751,7 +8750,7 @@
       <c r="D17" s="24"/>
       <c r="E17" s="24"/>
       <c r="F17" s="24">
-        <v>8888</v>
+        <v>88888</v>
       </c>
       <c r="G17" s="24"/>
       <c r="H17" s="24"/>

</xml_diff>